<commit_message>
:sunny: Betadiversity functions and maps
</commit_message>
<xml_diff>
--- a/input_data/Databases/Taxonomy_update_2021.xlsx
+++ b/input_data/Databases/Taxonomy_update_2021.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael\R_projects\ithomiini_diversity\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael\R_projects\ithomiini_diversity\input_data\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AEB10C-D5DD-40EF-8DB0-C1A5217A4319}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BFC9C2-8351-49D0-BA2B-03AB14859A4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{80E6AFEB-735A-4F48-B4E9-DF735B2EEC18}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taxonomy_update_2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -160,8 +160,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,16 +212,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A462DA-DC0B-45E6-9E55-8C03EB774F1F}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,321 +552,321 @@
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>